<commit_message>
State Table Outputs and Screen Clipping of Codes
The codes.png file has all of the information about input and output
formatting and encoding.  More progress on the output column.
</commit_message>
<xml_diff>
--- a/State Table.xlsx
+++ b/State Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="110">
   <si>
     <t>INPUT</t>
   </si>
@@ -312,6 +312,48 @@
   </si>
   <si>
     <t>1111-0100</t>
+  </si>
+  <si>
+    <t>0000-0011</t>
+  </si>
+  <si>
+    <t>0010-0011</t>
+  </si>
+  <si>
+    <t>0001-0010</t>
+  </si>
+  <si>
+    <t>0100-0000</t>
+  </si>
+  <si>
+    <t>1111-0011</t>
+  </si>
+  <si>
+    <t>0000-0101</t>
+  </si>
+  <si>
+    <t>1111-0101</t>
+  </si>
+  <si>
+    <t>0001-0100</t>
+  </si>
+  <si>
+    <t>0100-0010</t>
+  </si>
+  <si>
+    <t>0010-0100</t>
+  </si>
+  <si>
+    <t>1000-0010</t>
+  </si>
+  <si>
+    <t>0000-0110</t>
+  </si>
+  <si>
+    <t>0001-0101</t>
+  </si>
+  <si>
+    <t>0100-0011</t>
   </si>
 </sst>
 </file>
@@ -734,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="I224" sqref="I224"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1855,7 +1897,9 @@
       <c r="E38" s="4">
         <v>0.75</v>
       </c>
-      <c r="F38" s="13"/>
+      <c r="F38" s="13" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
@@ -1873,7 +1917,9 @@
       <c r="E39" s="4">
         <v>0.5</v>
       </c>
-      <c r="F39" s="13"/>
+      <c r="F39" s="13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
@@ -1891,7 +1937,9 @@
       <c r="E40" s="4">
         <v>0.25</v>
       </c>
-      <c r="F40" s="13"/>
+      <c r="F40" s="13" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
@@ -1909,7 +1957,9 @@
       <c r="E41" s="4">
         <v>0</v>
       </c>
-      <c r="F41" s="13"/>
+      <c r="F41" s="13" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
@@ -1927,7 +1977,9 @@
       <c r="E42" s="4">
         <v>0.75</v>
       </c>
-      <c r="F42" s="13"/>
+      <c r="F42" s="13" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
@@ -1945,7 +1997,9 @@
       <c r="E43" s="4">
         <v>0</v>
       </c>
-      <c r="F43" s="13"/>
+      <c r="F43" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
@@ -1963,7 +2017,9 @@
       <c r="E44" s="4">
         <v>1.25</v>
       </c>
-      <c r="F44" s="13"/>
+      <c r="F44" s="13" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
@@ -1981,7 +2037,9 @@
       <c r="E45" s="4">
         <v>1</v>
       </c>
-      <c r="F45" s="13"/>
+      <c r="F45" s="13" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
@@ -1999,7 +2057,9 @@
       <c r="E46" s="4">
         <v>0.75</v>
       </c>
-      <c r="F46" s="13"/>
+      <c r="F46" s="13" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
@@ -2017,7 +2077,9 @@
       <c r="E47" s="4">
         <v>0.5</v>
       </c>
-      <c r="F47" s="13"/>
+      <c r="F47" s="13" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
@@ -2035,7 +2097,9 @@
       <c r="E48" s="4">
         <v>0.25</v>
       </c>
-      <c r="F48" s="13"/>
+      <c r="F48" s="13" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
@@ -2053,7 +2117,9 @@
       <c r="E49" s="4">
         <v>0</v>
       </c>
-      <c r="F49" s="13"/>
+      <c r="F49" s="13" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
@@ -2071,7 +2137,9 @@
       <c r="E50" s="4">
         <v>0.5</v>
       </c>
-      <c r="F50" s="10"/>
+      <c r="F50" s="10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
@@ -2089,7 +2157,9 @@
       <c r="E51" s="4">
         <v>0.25</v>
       </c>
-      <c r="F51" s="10"/>
+      <c r="F51" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
@@ -2107,7 +2177,9 @@
       <c r="E52" s="4">
         <v>0</v>
       </c>
-      <c r="F52" s="10"/>
+      <c r="F52" s="10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
@@ -2125,7 +2197,9 @@
       <c r="E53" s="4">
         <v>0.5</v>
       </c>
-      <c r="F53" s="10"/>
+      <c r="F53" s="10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
@@ -2143,7 +2217,9 @@
       <c r="E54" s="4">
         <v>0.5</v>
       </c>
-      <c r="F54" s="10"/>
+      <c r="F54" s="10" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
@@ -2161,7 +2237,9 @@
       <c r="E55" s="4">
         <v>0</v>
       </c>
-      <c r="F55" s="10"/>
+      <c r="F55" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
@@ -2179,7 +2257,9 @@
       <c r="E56" s="4">
         <v>0.75</v>
       </c>
-      <c r="F56" s="10"/>
+      <c r="F56" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
@@ -2197,7 +2277,9 @@
       <c r="E57" s="4">
         <v>0.5</v>
       </c>
-      <c r="F57" s="10"/>
+      <c r="F57" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
@@ -2215,7 +2297,9 @@
       <c r="E58" s="4">
         <v>0.25</v>
       </c>
-      <c r="F58" s="10"/>
+      <c r="F58" s="10" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
@@ -2233,7 +2317,9 @@
       <c r="E59" s="4">
         <v>0</v>
       </c>
-      <c r="F59" s="10"/>
+      <c r="F59" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
@@ -2249,9 +2335,11 @@
         <v>23</v>
       </c>
       <c r="E60" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F60" s="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
@@ -2269,7 +2357,9 @@
       <c r="E61" s="4">
         <v>0</v>
       </c>
-      <c r="F61" s="10"/>
+      <c r="F61" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
@@ -2287,7 +2377,9 @@
       <c r="E62" s="4">
         <v>1</v>
       </c>
-      <c r="F62" s="10"/>
+      <c r="F62" s="10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
@@ -2305,7 +2397,9 @@
       <c r="E63" s="4">
         <v>0.75</v>
       </c>
-      <c r="F63" s="10"/>
+      <c r="F63" s="10" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
@@ -2323,7 +2417,9 @@
       <c r="E64" s="4">
         <v>0.5</v>
       </c>
-      <c r="F64" s="10"/>
+      <c r="F64" s="10" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
@@ -2341,7 +2437,9 @@
       <c r="E65" s="4">
         <v>0.25</v>
       </c>
-      <c r="F65" s="10"/>
+      <c r="F65" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
@@ -2359,7 +2457,9 @@
       <c r="E66" s="4">
         <v>0</v>
       </c>
-      <c r="F66" s="10"/>
+      <c r="F66" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
@@ -2377,7 +2477,9 @@
       <c r="E67" s="4">
         <v>0</v>
       </c>
-      <c r="F67" s="10"/>
+      <c r="F67" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
@@ -2395,7 +2497,9 @@
       <c r="E68" s="4">
         <v>1.5</v>
       </c>
-      <c r="F68" s="10"/>
+      <c r="F68" s="10" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
@@ -2413,7 +2517,9 @@
       <c r="E69" s="4">
         <v>1.25</v>
       </c>
-      <c r="F69" s="10"/>
+      <c r="F69" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
@@ -2431,7 +2537,9 @@
       <c r="E70" s="4">
         <v>1</v>
       </c>
-      <c r="F70" s="10"/>
+      <c r="F70" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
@@ -2449,7 +2557,9 @@
       <c r="E71" s="4">
         <v>0.75</v>
       </c>
-      <c r="F71" s="10"/>
+      <c r="F71" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
@@ -2467,7 +2577,9 @@
       <c r="E72" s="4">
         <v>0.5</v>
       </c>
-      <c r="F72" s="10"/>
+      <c r="F72" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
@@ -2485,7 +2597,9 @@
       <c r="E73" s="4">
         <v>0</v>
       </c>
-      <c r="F73" s="10"/>
+      <c r="F73" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">

</xml_diff>

<commit_message>
Debouncers + Some state work
</commit_message>
<xml_diff>
--- a/State Table.xlsx
+++ b/State Table.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -988,15 +987,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1084,6 +1074,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9174,7 +9173,7 @@
   <dimension ref="A1:U409"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20:K21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9200,35 +9199,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="87" t="s">
         <v>110</v>
       </c>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="88" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="39">
@@ -9249,27 +9248,27 @@
       <c r="G2" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="92" t="s">
+      <c r="H2" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="K2" s="76"/>
-      <c r="L2" s="75" t="s">
+      <c r="K2" s="112"/>
+      <c r="L2" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="77"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="75" t="s">
+      <c r="M2" s="111"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="110" t="s">
         <v>115</v>
       </c>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="76"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="112"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="88" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="39">
@@ -9290,7 +9289,7 @@
       <c r="G3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="89" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="60" t="s">
@@ -9299,13 +9298,13 @@
       <c r="K3" s="61">
         <v>0</v>
       </c>
-      <c r="L3" s="78" t="s">
+      <c r="L3" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="79" t="s">
+      <c r="M3" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="N3" s="81" t="s">
+      <c r="N3" s="78" t="s">
         <v>80</v>
       </c>
       <c r="O3" s="70" t="s">
@@ -9322,7 +9321,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="88" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="39">
@@ -9343,7 +9342,7 @@
       <c r="G4" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="92" t="s">
+      <c r="H4" s="89" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="60" t="s">
@@ -9375,7 +9374,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="88" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="39">
@@ -9396,7 +9395,7 @@
       <c r="G5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="92" t="s">
+      <c r="H5" s="89" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="60" t="s">
@@ -9428,7 +9427,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="90" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="42">
@@ -9449,7 +9448,7 @@
       <c r="G6" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="94" t="s">
+      <c r="H6" s="91" t="s">
         <v>11</v>
       </c>
       <c r="J6" s="60" t="s">
@@ -9481,7 +9480,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="88" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="39">
@@ -9502,7 +9501,7 @@
       <c r="G7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="89" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="60" t="s">
@@ -9534,7 +9533,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="88" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="39">
@@ -9555,13 +9554,13 @@
       <c r="G8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="92" t="s">
+      <c r="H8" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="K8" s="76"/>
+      <c r="K8" s="112"/>
       <c r="L8" s="62" t="s">
         <v>22</v>
       </c>
@@ -9585,7 +9584,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="88" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="39">
@@ -9606,19 +9605,19 @@
       <c r="G9" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="92" t="s">
+      <c r="H9" s="89" t="s">
         <v>70</v>
       </c>
       <c r="J9" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="80" t="s">
+      <c r="K9" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="75" t="s">
+      <c r="L9" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="76"/>
+      <c r="M9" s="112"/>
       <c r="N9" s="4"/>
       <c r="O9" s="60" t="s">
         <v>26</v>
@@ -9634,7 +9633,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="88" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="39">
@@ -9655,7 +9654,7 @@
       <c r="G10" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="92" t="s">
+      <c r="H10" s="89" t="s">
         <v>71</v>
       </c>
       <c r="J10" s="63" t="s">
@@ -9684,7 +9683,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="88" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="39">
@@ -9705,7 +9704,7 @@
       <c r="G11" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="92" t="s">
+      <c r="H11" s="89" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="64" t="s">
@@ -9734,7 +9733,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="92" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="47">
@@ -9755,7 +9754,7 @@
       <c r="G12" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="96" t="s">
+      <c r="H12" s="93" t="s">
         <v>11</v>
       </c>
       <c r="L12" s="60" t="s">
@@ -9774,7 +9773,7 @@
       <c r="R12" s="66"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="94" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="39">
@@ -9795,7 +9794,7 @@
       <c r="G13" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="98" t="s">
+      <c r="H13" s="95" t="s">
         <v>13</v>
       </c>
       <c r="L13" s="60" t="s">
@@ -9807,7 +9806,7 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="94" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="39">
@@ -9828,7 +9827,7 @@
       <c r="G14" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="98" t="s">
+      <c r="H14" s="95" t="s">
         <v>70</v>
       </c>
       <c r="L14" s="60" t="s">
@@ -9840,7 +9839,7 @@
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="94" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="39">
@@ -9861,10 +9860,10 @@
       <c r="G15" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="98" t="s">
+      <c r="H15" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="85" t="s">
+      <c r="J15" s="82" t="s">
         <v>116</v>
       </c>
       <c r="L15" s="60" t="s">
@@ -9876,7 +9875,7 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="94" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="39">
@@ -9897,10 +9896,10 @@
       <c r="G16" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="98" t="s">
+      <c r="H16" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="82" t="s">
+      <c r="J16" s="79" t="s">
         <v>117</v>
       </c>
       <c r="L16" s="60" t="s">
@@ -9912,7 +9911,7 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="94" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="39">
@@ -9933,10 +9932,10 @@
       <c r="G17" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="98" t="s">
+      <c r="H17" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="83" t="s">
+      <c r="J17" s="80" t="s">
         <v>118</v>
       </c>
       <c r="L17" s="60" t="s">
@@ -9948,7 +9947,7 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="99" t="s">
+      <c r="A18" s="96" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="45">
@@ -9969,10 +9968,10 @@
       <c r="G18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="100" t="s">
+      <c r="H18" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="84" t="s">
+      <c r="J18" s="81" t="s">
         <v>119</v>
       </c>
       <c r="L18" s="62" t="s">
@@ -9984,7 +9983,7 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="98" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="47">
@@ -10005,7 +10004,7 @@
       <c r="G19" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="96" t="s">
+      <c r="H19" s="93" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="1"/>
@@ -10014,7 +10013,7 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="94" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="39">
@@ -10035,14 +10034,14 @@
       <c r="G20" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="98" t="s">
+      <c r="H20" s="95" t="s">
         <v>70</v>
       </c>
       <c r="I20" s="1"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="97" t="s">
+      <c r="A21" s="94" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="39">
@@ -10063,13 +10062,13 @@
       <c r="G21" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="98" t="s">
+      <c r="H21" s="95" t="s">
         <v>14</v>
       </c>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="97" t="s">
+      <c r="A22" s="94" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="39">
@@ -10090,13 +10089,13 @@
       <c r="G22" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="95" t="s">
         <v>71</v>
       </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="97" t="s">
+      <c r="A23" s="94" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="39">
@@ -10117,13 +10116,13 @@
       <c r="G23" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="98" t="s">
+      <c r="H23" s="95" t="s">
         <v>73</v>
       </c>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="97" t="s">
+      <c r="A24" s="94" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="39">
@@ -10144,13 +10143,13 @@
       <c r="G24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="98" t="s">
+      <c r="H24" s="95" t="s">
         <v>70</v>
       </c>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="96" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="45">
@@ -10171,13 +10170,13 @@
       <c r="G25" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="100" t="s">
+      <c r="H25" s="97" t="s">
         <v>13</v>
       </c>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="99" t="s">
+      <c r="A26" s="96" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="45">
@@ -10198,13 +10197,13 @@
       <c r="G26" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="100" t="s">
+      <c r="H26" s="97" t="s">
         <v>12</v>
       </c>
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="102" t="s">
+      <c r="A27" s="99" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="47">
@@ -10225,13 +10224,13 @@
       <c r="G27" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="103" t="s">
+      <c r="H27" s="100" t="s">
         <v>11</v>
       </c>
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="94" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="39">
@@ -10252,13 +10251,13 @@
       <c r="G28" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="98" t="s">
+      <c r="H28" s="95" t="s">
         <v>14</v>
       </c>
       <c r="N28" s="4"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="97" t="s">
+      <c r="A29" s="94" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="39">
@@ -10279,13 +10278,13 @@
       <c r="G29" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="98" t="s">
+      <c r="H29" s="95" t="s">
         <v>71</v>
       </c>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="97" t="s">
+      <c r="A30" s="94" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="39">
@@ -10306,14 +10305,14 @@
       <c r="G30" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="98" t="s">
+      <c r="H30" s="95" t="s">
         <v>72</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="97" t="s">
+      <c r="A31" s="94" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="39">
@@ -10334,12 +10333,12 @@
       <c r="G31" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="98" t="s">
+      <c r="H31" s="95" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="97" t="s">
+      <c r="A32" s="94" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="39">
@@ -10360,12 +10359,12 @@
       <c r="G32" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="98" t="s">
+      <c r="H32" s="95" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="101" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="45">
@@ -10386,12 +10385,12 @@
       <c r="G33" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="100" t="s">
+      <c r="H33" s="97" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="101" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="45">
@@ -10412,12 +10411,12 @@
       <c r="G34" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="100" t="s">
+      <c r="H34" s="97" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="104" t="s">
+      <c r="A35" s="101" t="s">
         <v>25</v>
       </c>
       <c r="B35" s="45">
@@ -10438,12 +10437,12 @@
       <c r="G35" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="100" t="s">
+      <c r="H35" s="97" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="95" t="s">
+      <c r="A36" s="92" t="s">
         <v>25</v>
       </c>
       <c r="B36" s="47">
@@ -10464,12 +10463,12 @@
       <c r="G36" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="103" t="s">
+      <c r="H36" s="100" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="94" t="s">
         <v>26</v>
       </c>
       <c r="B37" s="39">
@@ -10490,12 +10489,12 @@
       <c r="G37" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="98" t="s">
+      <c r="H37" s="95" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="94" t="s">
         <v>26</v>
       </c>
       <c r="B38" s="39">
@@ -10516,12 +10515,12 @@
       <c r="G38" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="98" t="s">
+      <c r="H38" s="95" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="97" t="s">
+      <c r="A39" s="94" t="s">
         <v>26</v>
       </c>
       <c r="B39" s="39">
@@ -10542,12 +10541,12 @@
       <c r="G39" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="98" t="s">
+      <c r="H39" s="95" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="105" t="s">
+      <c r="A40" s="102" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="36">
@@ -10566,10 +10565,10 @@
       <c r="G40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="106"/>
+      <c r="H40" s="103"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="97" t="s">
+      <c r="A41" s="94" t="s">
         <v>26</v>
       </c>
       <c r="B41" s="39">
@@ -10590,12 +10589,12 @@
       <c r="G41" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="98" t="s">
+      <c r="H41" s="95" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="104" t="s">
+      <c r="A42" s="101" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="45">
@@ -10616,12 +10615,12 @@
       <c r="G42" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="100" t="s">
+      <c r="H42" s="97" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="104" t="s">
+      <c r="A43" s="101" t="s">
         <v>26</v>
       </c>
       <c r="B43" s="45">
@@ -10642,12 +10641,12 @@
       <c r="G43" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="100" t="s">
+      <c r="H43" s="97" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="104" t="s">
+      <c r="A44" s="101" t="s">
         <v>26</v>
       </c>
       <c r="B44" s="45">
@@ -10668,12 +10667,12 @@
       <c r="G44" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="100" t="s">
+      <c r="H44" s="97" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="95" t="s">
+      <c r="A45" s="92" t="s">
         <v>26</v>
       </c>
       <c r="B45" s="47">
@@ -10694,12 +10693,12 @@
       <c r="G45" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="103" t="s">
+      <c r="H45" s="100" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="97" t="s">
+      <c r="A46" s="94" t="s">
         <v>27</v>
       </c>
       <c r="B46" s="39">
@@ -10720,12 +10719,12 @@
       <c r="G46" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="98" t="s">
+      <c r="H46" s="95" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="97" t="s">
+      <c r="A47" s="94" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="39">
@@ -10746,12 +10745,12 @@
       <c r="G47" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="98" t="s">
+      <c r="H47" s="95" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="97" t="s">
+      <c r="A48" s="94" t="s">
         <v>27</v>
       </c>
       <c r="B48" s="39">
@@ -10772,12 +10771,12 @@
       <c r="G48" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H48" s="98" t="s">
+      <c r="H48" s="95" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="105" t="s">
+      <c r="A49" s="102" t="s">
         <v>27</v>
       </c>
       <c r="B49" s="36">
@@ -10796,10 +10795,10 @@
       <c r="G49" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H49" s="106"/>
+      <c r="H49" s="103"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="97" t="s">
+      <c r="A50" s="94" t="s">
         <v>27</v>
       </c>
       <c r="B50" s="39">
@@ -10820,12 +10819,12 @@
       <c r="G50" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="98" t="s">
+      <c r="H50" s="95" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="104" t="s">
+      <c r="A51" s="101" t="s">
         <v>27</v>
       </c>
       <c r="B51" s="45">
@@ -10846,12 +10845,12 @@
       <c r="G51" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="100" t="s">
+      <c r="H51" s="97" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="104" t="s">
+      <c r="A52" s="101" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="45">
@@ -10872,12 +10871,12 @@
       <c r="G52" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="100" t="s">
+      <c r="H52" s="97" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="104" t="s">
+      <c r="A53" s="101" t="s">
         <v>27</v>
       </c>
       <c r="B53" s="45">
@@ -10898,12 +10897,12 @@
       <c r="G53" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H53" s="100" t="s">
+      <c r="H53" s="97" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="95" t="s">
+      <c r="A54" s="92" t="s">
         <v>27</v>
       </c>
       <c r="B54" s="47">
@@ -10924,12 +10923,12 @@
       <c r="G54" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="H54" s="103" t="s">
+      <c r="H54" s="100" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="97" t="s">
+      <c r="A55" s="94" t="s">
         <v>28</v>
       </c>
       <c r="B55" s="39">
@@ -10950,12 +10949,12 @@
       <c r="G55" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H55" s="98" t="s">
+      <c r="H55" s="95" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="97" t="s">
+      <c r="A56" s="94" t="s">
         <v>28</v>
       </c>
       <c r="B56" s="39">
@@ -10976,12 +10975,12 @@
       <c r="G56" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H56" s="98" t="s">
+      <c r="H56" s="95" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="105" t="s">
+      <c r="A57" s="102" t="s">
         <v>28</v>
       </c>
       <c r="B57" s="36">
@@ -11000,10 +10999,10 @@
       <c r="G57" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H57" s="106"/>
+      <c r="H57" s="103"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="105" t="s">
+      <c r="A58" s="102" t="s">
         <v>28</v>
       </c>
       <c r="B58" s="36">
@@ -11022,10 +11021,10 @@
       <c r="G58" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="106"/>
+      <c r="H58" s="103"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="97" t="s">
+      <c r="A59" s="94" t="s">
         <v>28</v>
       </c>
       <c r="B59" s="39">
@@ -11046,12 +11045,12 @@
       <c r="G59" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H59" s="98" t="s">
+      <c r="H59" s="95" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="104" t="s">
+      <c r="A60" s="101" t="s">
         <v>28</v>
       </c>
       <c r="B60" s="45">
@@ -11072,12 +11071,12 @@
       <c r="G60" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H60" s="100" t="s">
+      <c r="H60" s="97" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="104" t="s">
+      <c r="A61" s="101" t="s">
         <v>28</v>
       </c>
       <c r="B61" s="45">
@@ -11098,12 +11097,12 @@
       <c r="G61" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H61" s="100" t="s">
+      <c r="H61" s="97" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="104" t="s">
+      <c r="A62" s="101" t="s">
         <v>28</v>
       </c>
       <c r="B62" s="45">
@@ -11124,12 +11123,12 @@
       <c r="G62" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="100" t="s">
+      <c r="H62" s="97" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="95" t="s">
+      <c r="A63" s="92" t="s">
         <v>28</v>
       </c>
       <c r="B63" s="47">
@@ -11150,12 +11149,12 @@
       <c r="G63" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="103" t="s">
+      <c r="H63" s="100" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="97" t="s">
+      <c r="A64" s="94" t="s">
         <v>29</v>
       </c>
       <c r="B64" s="39">
@@ -11176,12 +11175,12 @@
       <c r="G64" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H64" s="98" t="s">
+      <c r="H64" s="95" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="105" t="s">
+      <c r="A65" s="102" t="s">
         <v>29</v>
       </c>
       <c r="B65" s="36">
@@ -11200,10 +11199,10 @@
       <c r="G65" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H65" s="106"/>
+      <c r="H65" s="103"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="105" t="s">
+      <c r="A66" s="102" t="s">
         <v>29</v>
       </c>
       <c r="B66" s="36">
@@ -11222,10 +11221,10 @@
       <c r="G66" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="106"/>
+      <c r="H66" s="103"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="105" t="s">
+      <c r="A67" s="102" t="s">
         <v>29</v>
       </c>
       <c r="B67" s="36">
@@ -11244,10 +11243,10 @@
       <c r="G67" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H67" s="106"/>
+      <c r="H67" s="103"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="97" t="s">
+      <c r="A68" s="94" t="s">
         <v>29</v>
       </c>
       <c r="B68" s="39">
@@ -11268,12 +11267,12 @@
       <c r="G68" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H68" s="98" t="s">
+      <c r="H68" s="95" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="104" t="s">
+      <c r="A69" s="101" t="s">
         <v>29</v>
       </c>
       <c r="B69" s="45">
@@ -11294,12 +11293,12 @@
       <c r="G69" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="100" t="s">
+      <c r="H69" s="97" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="104" t="s">
+      <c r="A70" s="101" t="s">
         <v>29</v>
       </c>
       <c r="B70" s="45">
@@ -11320,12 +11319,12 @@
       <c r="G70" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="H70" s="100" t="s">
+      <c r="H70" s="97" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="104" t="s">
+      <c r="A71" s="101" t="s">
         <v>29</v>
       </c>
       <c r="B71" s="45">
@@ -11346,33 +11345,33 @@
       <c r="G71" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H71" s="100" t="s">
+      <c r="H71" s="97" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="107" t="s">
+      <c r="A72" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="B72" s="108">
+      <c r="B72" s="105">
         <v>2</v>
       </c>
-      <c r="C72" s="109" t="s">
+      <c r="C72" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="110" t="s">
+      <c r="D72" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="111" t="s">
+      <c r="E72" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="F72" s="108">
+      <c r="F72" s="105">
         <v>1</v>
       </c>
-      <c r="G72" s="109" t="s">
+      <c r="G72" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="H72" s="112" t="s">
+      <c r="H72" s="109" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>